<commit_message>
checkout test report updated
</commit_message>
<xml_diff>
--- a/NopCommerce/Test_Reports/TC_CheckOut_Report .xlsx
+++ b/NopCommerce/Test_Reports/TC_CheckOut_Report .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_Projects\NopCommerce\TestBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_Projects\NopCommerce\Test_Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -42,30 +42,105 @@
     <t>TC_01</t>
   </si>
   <si>
-    <t>TC_02</t>
-  </si>
-  <si>
     <t>TC_03</t>
   </si>
   <si>
-    <t>Go to checkout but by registering new account</t>
-  </si>
-  <si>
-    <t>Go to checkout using registered account (Log in)</t>
-  </si>
-  <si>
-    <t>Go to checkout using (Checkout as a guest) option</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>thatshouldmakeit</t>
+  </si>
+  <si>
+    <t>CorrectEmail13@gmail.com</t>
+  </si>
+  <si>
+    <t>correctEmail22@gmail.com</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Head Office, Plot No. 8471, PACRA House Haile Selassie Avenue</t>
+  </si>
+  <si>
+    <t>44 Elmessaha Street. Dokki, Giza</t>
+  </si>
+  <si>
+    <t>Zip/postal code</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>(260 211) 255 151</t>
+  </si>
+  <si>
+    <t>02 333 66 547</t>
+  </si>
+  <si>
+    <t>Shipping method</t>
+  </si>
+  <si>
+    <t>Next Day Air</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Payment option</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Order Successfully added</t>
+  </si>
+  <si>
+    <t>Register new accout -&gt; login -&gt; add item to cart-&gt; go to checkout</t>
+  </si>
+  <si>
+    <t>add item to cart -&gt; go to checkout as a guest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -91,6 +166,14 @@
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -137,10 +220,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -157,8 +241,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,23 +549,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="98.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="36.125" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="26.25" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="29.25" customWidth="1"/>
+    <col min="10" max="10" width="16.625" customWidth="1"/>
+    <col min="11" max="13" width="20.375" customWidth="1"/>
+    <col min="14" max="14" width="38" customWidth="1"/>
+    <col min="15" max="15" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.125" customWidth="1"/>
+    <col min="17" max="17" width="98.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,59 +582,154 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:17" ht="33.75" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3">
+        <v>12611</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:17" ht="50.25" customHeight="1" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10101</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="4"/>
+    <row r="12" spans="1:17">
+      <c r="N12" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="CorrectEmail@gmail.com"/>
+    <hyperlink ref="J3" r:id="rId2" display="https://www.google.com/search?sca_esv=db94807e8ff0f820&amp;sxsrf=ADLYWIIoPZy-X6tkf-uJxurfG5JZk3jcNA:1716892109518&amp;q=lusaka+10101&amp;stick=H4sIAAAAAAAAAONgVuLVT9c3NKw0jDcqNE_PesRowS3w8sc9YSn9SWtOXmPU5OIKzsgvd80rySypFJLmYoOyBKX4uVB18ixi5ckpLU7MTlQwNABCANKFF65bAAAA&amp;sa=X&amp;ved=2ahUKEwixvLjCkbCGAxWVA9sEHTdnDd0QzIcDKAB6BAglEAE"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>